<commit_message>
Added Main, Acem login, login diagram and config file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandra.veizu\Documents\Reframework_update_UiPath_Services\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/971dc324aecf299b/Documents/UiPath/RoboticEnterpriseFramework1/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8A59F621-EEF1-4DAA-A001-E1301CB4CB83}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -88,10 +88,6 @@
   </si>
   <si>
     <t>Framework</t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -102,33 +98,77 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>downloadBaseFolderPath</t>
+  </si>
+  <si>
+    <t>workingDirectory</t>
+  </si>
+  <si>
+    <t>Ingrid</t>
+  </si>
+  <si>
+    <t>Updated at runtime constitutes of today's day and time for which the bot is running</t>
+  </si>
+  <si>
+    <t>Maximum wait value before an error is thrown while downloading a file</t>
+  </si>
+  <si>
+    <t>t01_IngridFacebookCredentials</t>
+  </si>
+  <si>
+    <t>facebookCredentials</t>
+  </si>
+  <si>
+    <t>Name of assest credentials which will be used for Facebook at runtime</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>acmeUrl</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/login</t>
+  </si>
+  <si>
+    <t>acmeWI5Queue</t>
+  </si>
+  <si>
+    <t>Acme WI5</t>
+  </si>
+  <si>
+    <t>acmeCredentials</t>
+  </si>
+  <si>
+    <t>WI5AcmeCredentials</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -152,6 +192,18 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF485056"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -170,10 +222,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -183,8 +236,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -500,7 +556,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -547,55 +603,102 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
+    <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="2:2" ht="14.25" customHeight="1">
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="19" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="2:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1563,8 +1666,11 @@
     <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{9428091E-8EC3-41E9-8E1A-6DE40D3D28E8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1572,7 +1678,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -1624,7 +1732,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1648,7 +1756,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1670,7 +1778,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1681,7 +1789,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1692,7 +1800,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2683,7 +2791,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C2"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2702,7 +2810,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2730,7 +2838,11 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3732,5 +3844,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the following files: Filter_Work_Items_DataTable and Add_Working_Items_To_Queue
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/971dc324aecf299b/Documents/UiPath/RoboticEnterpriseFramework1/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olmcc\Documents\UiPath\uipath_t05_AcmeSystemsWI5\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8A59F621-EEF1-4DAA-A001-E1301CB4CB83}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE09826-6F19-4DD4-BCB9-72A52258BD01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -162,6 +159,18 @@
   </si>
   <si>
     <t>WI5AcmeCredentials</t>
+  </si>
+  <si>
+    <t>http://www.sha1-online.com/</t>
+  </si>
+  <si>
+    <t>shaURL</t>
+  </si>
+  <si>
+    <t>Acme Wi5 Hash Generator</t>
+  </si>
+  <si>
+    <t>timeOutValue</t>
   </si>
 </sst>
 </file>
@@ -226,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -238,6 +247,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -553,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -603,13 +615,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -617,61 +629,61 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
         <v>36</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
         <v>42</v>
-      </c>
-      <c r="B9" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -680,25 +692,25 @@
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="2:2" ht="14.25" customHeight="1">
-      <c r="B17" s="6"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B16" s="6"/>
     </row>
-    <row r="18" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="19" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="20" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="22" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="23" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="24" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="25" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="26" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="27" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="28" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="17" ht="14.25" customHeight="1"/>
+    <row r="18" ht="14.25" customHeight="1"/>
+    <row r="19" ht="14.25" customHeight="1"/>
+    <row r="20" ht="14.25" customHeight="1"/>
+    <row r="21" ht="14.25" customHeight="1"/>
+    <row r="22" ht="14.25" customHeight="1"/>
+    <row r="23" ht="14.25" customHeight="1"/>
+    <row r="24" ht="14.25" customHeight="1"/>
+    <row r="25" ht="14.25" customHeight="1"/>
+    <row r="26" ht="14.25" customHeight="1"/>
+    <row r="27" ht="14.25" customHeight="1"/>
+    <row r="28" ht="14.25" customHeight="1"/>
+    <row r="29" ht="14.25" customHeight="1"/>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="32" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1663,14 +1675,14 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" xr:uid="{9428091E-8EC3-41E9-8E1A-6DE40D3D28E8}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{7A0AF8E1-4569-45A5-8922-9FC43DD0B90A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1679,7 +1691,7 @@
   <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1732,7 +1744,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1756,7 +1768,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1778,7 +1790,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1789,7 +1801,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1800,10 +1812,17 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="7">
+        <v>3.3564814814814812E-4</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2790,8 +2809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2810,7 +2829,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2839,8 +2858,14 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
removed log message that was created for testing retry
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olmcc\Documents\UiPath\uipath_t05_AcmeSystemsWI5\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2845EDE0-58CB-435D-AB74-F0A3617A7C89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DE957D-3F22-47BB-8530-12FB27B0349A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3525" yWindow="3375" windowWidth="23100" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2805" yWindow="210" windowWidth="23100" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -570,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1700,7 +1700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -2871,12 +2871,7 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="D2" t="s">
         <v>33</v>
       </c>

</xml_diff>